<commit_message>
got stock contracts working, if inelegantly.
</commit_message>
<xml_diff>
--- a/data/other/AlgoStockContact.xlsx
+++ b/data/other/AlgoStockContact.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/90b86913ab8efd7b/Desktop/bitburner/data/other/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/90b86913ab8efd7b/Desktop/bitburner/bitburner/data/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="453" documentId="8_{5709C273-8E06-45BC-94A8-2BE9F3E1B853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CA3E678-7F2A-4AEF-93E8-E0494516745B}"/>
+  <xr:revisionPtr revIDLastSave="474" documentId="8_{5709C273-8E06-45BC-94A8-2BE9F3E1B853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2244D8C-BA25-40D5-AF86-7C5C5643DB8D}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15960" windowWidth="29040" windowHeight="15720" xr2:uid="{478B04DD-BDD8-4F1D-84B5-0F5206477317}"/>
   </bookViews>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785A79B2-97EF-4992-BCB4-B2DBC9CAED3C}">
   <dimension ref="A2:AA63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="U50" sqref="U50"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,7 +456,7 @@
     <col min="1" max="1" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -503,7 +503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -545,7 +545,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D4">
         <f>D3-C3</f>
         <v>80</v>
@@ -582,7 +582,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="I5">
         <f>I3-E3</f>
         <v>127</v>
@@ -603,7 +603,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="P6">
         <v>4</v>
       </c>
@@ -616,7 +616,7 @@
         <v>10097</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="P7">
         <v>5</v>
       </c>
@@ -625,7 +625,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="P8">
         <v>6</v>
       </c>
@@ -634,66 +634,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="V9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>3</v>
-      </c>
-      <c r="O10">
-        <v>2</v>
-      </c>
-      <c r="P10">
-        <v>5</v>
-      </c>
-      <c r="Q10">
-        <v>4</v>
-      </c>
-      <c r="R10">
-        <v>6</v>
-      </c>
-      <c r="S10">
-        <v>3</v>
-      </c>
-      <c r="T10">
-        <v>100</v>
-      </c>
-      <c r="V10">
-        <v>1</v>
-      </c>
-      <c r="W10">
-        <f>T11</f>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="N11">
-        <v>2</v>
-      </c>
-      <c r="P11">
-        <v>4</v>
-      </c>
-      <c r="R11">
-        <v>5</v>
-      </c>
-      <c r="T11">
-        <v>99</v>
-      </c>
-      <c r="V11">
-        <v>2</v>
-      </c>
-      <c r="W11">
-        <f>T11+R11+U12</f>
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -712,31 +653,8 @@
       <c r="H12" t="s">
         <v>10</v>
       </c>
-      <c r="R12">
-        <f>R10-Q10</f>
-        <v>2</v>
-      </c>
-      <c r="S12">
-        <f>R12-R11</f>
-        <v>-3</v>
-      </c>
-      <c r="T12">
-        <f>T10-S10</f>
-        <v>97</v>
-      </c>
-      <c r="U12">
-        <f>T12-T11</f>
-        <v>-2</v>
-      </c>
-      <c r="V12">
-        <v>3</v>
-      </c>
-      <c r="W12">
-        <f>T11+R11+P11+U12+S12</f>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -752,11 +670,8 @@
       <c r="H13" t="s">
         <v>10</v>
       </c>
-      <c r="V13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>6</v>
       </c>
@@ -773,7 +688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>7</v>
       </c>
@@ -790,7 +705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>7</v>
       </c>
@@ -1108,12 +1023,12 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:22" x14ac:dyDescent="0.35">
       <c r="O33">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:22" x14ac:dyDescent="0.35">
       <c r="O34">
         <v>6</v>
       </c>
@@ -1122,7 +1037,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="35" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T35">
         <v>131</v>
       </c>
@@ -1134,7 +1049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T36">
         <v>64</v>
       </c>
@@ -1146,7 +1061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T37">
         <v>35</v>
       </c>
@@ -1158,7 +1073,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T38">
         <v>6</v>
       </c>
@@ -1170,7 +1085,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T39">
         <v>122</v>
       </c>
@@ -1182,7 +1097,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T40">
         <v>38</v>
       </c>
@@ -1194,7 +1109,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T41">
         <v>47</v>
       </c>
@@ -1206,7 +1121,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T42">
         <v>50</v>
       </c>
@@ -1218,7 +1133,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T43">
         <v>12</v>
       </c>
@@ -1230,7 +1145,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T44">
         <v>10</v>
       </c>
@@ -1242,7 +1157,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T45">
         <v>35</v>
       </c>
@@ -1254,7 +1169,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T46">
         <v>22</v>
       </c>
@@ -1266,7 +1181,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:22" x14ac:dyDescent="0.35">
       <c r="T47">
         <v>40</v>
       </c>
@@ -1278,7 +1193,10 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="15:22" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:22" x14ac:dyDescent="0.35">
+      <c r="J48" t="s">
+        <v>0</v>
+      </c>
       <c r="T48">
         <v>10</v>
       </c>
@@ -1290,7 +1208,38 @@
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>6</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <v>100</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <f>H50</f>
+        <v>99</v>
+      </c>
       <c r="T49">
         <v>92</v>
       </c>
@@ -1302,85 +1251,193 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <v>99</v>
+      </c>
+      <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <f>H50+F50+I51</f>
+        <v>102</v>
+      </c>
       <c r="V50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="F51">
+        <f>F49-E49</f>
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <f>F51-F50</f>
+        <v>-3</v>
+      </c>
+      <c r="H51">
+        <f>H49-G49</f>
+        <v>97</v>
+      </c>
+      <c r="I51">
+        <f>H51-H50</f>
+        <v>-2</v>
+      </c>
+      <c r="J51">
+        <v>3</v>
+      </c>
+      <c r="K51">
+        <f>H50+F50+D50+I51+G51</f>
+        <v>103</v>
+      </c>
       <c r="V51">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="J52">
+        <v>4</v>
+      </c>
       <c r="V52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
       <c r="V53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
       <c r="V54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
       <c r="V55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
       <c r="V56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
       <c r="V57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
       <c r="V58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
       <c r="V59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <f>F62</f>
+        <v>99</v>
+      </c>
       <c r="V60">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>5</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>100</v>
+      </c>
+      <c r="I61">
+        <v>2</v>
+      </c>
+      <c r="J61">
+        <f>F62+D62+G63</f>
+        <v>102</v>
+      </c>
       <c r="V61">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
+      <c r="F62">
+        <v>99</v>
+      </c>
+      <c r="I62">
+        <v>3</v>
+      </c>
+      <c r="J62">
+        <f>F62+D62+B62+E63+G63</f>
+        <v>103</v>
+      </c>
       <c r="V62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="20:22" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D63">
+        <f>D61-C61</f>
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <f>D63-D62</f>
+        <v>-1</v>
+      </c>
+      <c r="F63">
+        <v>98</v>
+      </c>
+      <c r="G63">
+        <f>F63-F62</f>
+        <v>-1</v>
+      </c>
       <c r="V63">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>